<commit_message>
Update, 250SPS, 3ch differential setup.
</commit_message>
<xml_diff>
--- a/Ads1299_defRegs.xlsx
+++ b/Ads1299_defRegs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmoodms\Documents\_APPDEV_new\nRF_Development\nRF5_SDK_11.0.0_2\examples\_my_projects\nRF51_EMG_ADS1299_3ch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahmood31\Google Drive\nRF5_SDK_11.0.0_2\examples\_my_projects\nRF51_EMG_ADS1299_3ch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -721,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>